<commit_message>
added more cards and some bug fixes
</commit_message>
<xml_diff>
--- a/Links.xlsx
+++ b/Links.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aditya\Projects\Portfolio\Practice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aditya\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECAFE94F-E17A-4B80-AE7F-B4531D3A458E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1156254A-2492-4D3C-BC0E-8662906BBC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0AE215CC-A1AB-4149-94F4-3B8936C851DB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="113">
   <si>
     <t>Energy Transition</t>
   </si>
@@ -240,9 +240,6 @@
   </si>
   <si>
     <t>https://india.mongabay.com/2023/10/poor-governance-burdens-indian-cities-finds-survey/</t>
-  </si>
-  <si>
-    <t>https://www.downtoearth.org.in/interviews/urbanisation/-green-roofs-can-help-cities-adapt-to-climate-change--50850</t>
   </si>
   <si>
     <t>https://india.mongabay.com/2023/07/community-based-natural-farming-outshines-other-farming-practices-in-andhra-pradesh-in-all-aspects/</t>
@@ -445,7 +442,38 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -777,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B6FFBC-4681-4669-B232-AC94051921B9}">
   <dimension ref="A4:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -836,13 +864,13 @@
         <v>66</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -862,13 +890,13 @@
         <v>67</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -888,13 +916,13 @@
         <v>30</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -910,17 +938,15 @@
       <c r="D8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>68</v>
-      </c>
+      <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -940,10 +966,10 @@
         <v>55</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -960,10 +986,10 @@
         <v>52</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -980,10 +1006,10 @@
         <v>53</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1000,10 +1026,10 @@
         <v>54</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -1020,10 +1046,10 @@
         <v>55</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1040,10 +1066,10 @@
         <v>56</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1060,10 +1086,10 @@
         <v>57</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1077,10 +1103,10 @@
         <v>58</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1094,10 +1120,10 @@
         <v>59</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1111,10 +1137,10 @@
         <v>60</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1128,10 +1154,10 @@
         <v>61</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1142,10 +1168,10 @@
         <v>62</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1156,7 +1182,7 @@
         <v>63</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H21" s="2"/>
     </row>
@@ -1165,7 +1191,7 @@
         <v>64</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -1173,40 +1199,46 @@
         <v>65</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G24" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G25" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G26" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G27" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G28" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G29" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:H29">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1" xr:uid="{6309066A-7C9F-4DEA-A9DD-A4AF05B10080}"/>
     <hyperlink ref="A6" r:id="rId2" xr:uid="{06D4A388-AF14-4BA2-A3D2-1D4586A44FE6}"/>
@@ -1273,54 +1305,54 @@
     <hyperlink ref="E5" r:id="rId63" xr:uid="{FDA5CE52-AB9E-4C9B-BE1E-DE0B2BD47688}"/>
     <hyperlink ref="E6" r:id="rId64" xr:uid="{CACCA0EF-174B-410E-8DE4-370EBB7AF83C}"/>
     <hyperlink ref="E7" r:id="rId65" xr:uid="{0A4CE24E-0552-41AB-9E12-1C93F8C5F2FE}"/>
-    <hyperlink ref="E8" r:id="rId66" xr:uid="{4E85C7A6-B815-4C38-A658-5E36647B9379}"/>
-    <hyperlink ref="F5" r:id="rId67" xr:uid="{355C9F80-5851-45EB-AA61-2D400AC39C40}"/>
-    <hyperlink ref="F6" r:id="rId68" xr:uid="{0C0516A7-7AC8-4132-A632-144B988DEDAC}"/>
-    <hyperlink ref="F7" r:id="rId69" xr:uid="{E0F2986D-CA81-4EA1-8548-DC7F377C2E79}"/>
-    <hyperlink ref="F8" r:id="rId70" xr:uid="{67BD70F3-ABE9-4C8F-AFB1-41B6D51FBAF6}"/>
-    <hyperlink ref="F9" r:id="rId71" xr:uid="{1AAEE675-B4FF-4FA3-83FA-7393FFBD697B}"/>
-    <hyperlink ref="G5" r:id="rId72" xr:uid="{363702E4-8A66-4A19-AA8F-679E22E89404}"/>
-    <hyperlink ref="G6" r:id="rId73" xr:uid="{BEDF7C13-C82E-4CB5-8860-6E9C089A3826}"/>
-    <hyperlink ref="G7" r:id="rId74" xr:uid="{C65C518A-17C5-4C37-B156-B294BB7C39DE}"/>
-    <hyperlink ref="G8" r:id="rId75" xr:uid="{1A08BA37-85E0-46EC-BE46-4CFF50561D88}"/>
-    <hyperlink ref="G9" r:id="rId76" xr:uid="{D1A6861C-9A60-441C-ACCE-9DA32723FD25}"/>
-    <hyperlink ref="G10" r:id="rId77" xr:uid="{BE83C08E-9EAE-4B29-B12C-7C6BEA71710E}"/>
-    <hyperlink ref="G11" r:id="rId78" xr:uid="{F9FADDBC-B865-49C2-8DA7-31DD7D450BB6}"/>
-    <hyperlink ref="G12" r:id="rId79" xr:uid="{455C45C1-E21D-47FC-831A-41CDD067DA7F}"/>
-    <hyperlink ref="G13" r:id="rId80" xr:uid="{3DA6D7C1-09B5-49C4-9B34-4316A05F2F32}"/>
-    <hyperlink ref="G14" r:id="rId81" xr:uid="{25178FE7-FA65-4469-B8FB-2CAB8F5A603E}"/>
-    <hyperlink ref="G15" r:id="rId82" xr:uid="{557D08BC-5C21-4FC3-9724-C76098698E3D}"/>
-    <hyperlink ref="G16" r:id="rId83" xr:uid="{9C0B4647-6398-46DE-91C5-D70A157EB87D}"/>
-    <hyperlink ref="G17" r:id="rId84" xr:uid="{EB927B41-C00C-4953-AD42-82B427AD4B72}"/>
-    <hyperlink ref="G18" r:id="rId85" xr:uid="{431D0FB1-AB5E-4AE5-A04A-24C256A2BF31}"/>
-    <hyperlink ref="G19" r:id="rId86" xr:uid="{F7251C95-65F3-4AEE-ABDA-2753B311B594}"/>
-    <hyperlink ref="G20" r:id="rId87" xr:uid="{F35454C0-EC02-4D31-B421-FAC25569AC72}"/>
-    <hyperlink ref="G21" r:id="rId88" xr:uid="{87E4AC5D-2E2F-47CD-9FC0-0E7825DE6414}"/>
-    <hyperlink ref="G22" r:id="rId89" xr:uid="{BF883CF3-071F-4584-A944-B0975E1EED1F}"/>
-    <hyperlink ref="G23" r:id="rId90" xr:uid="{B69207CB-3C13-484E-B116-78D83E9B50AC}"/>
-    <hyperlink ref="G24" r:id="rId91" xr:uid="{434F605D-D946-4CCC-AA04-39966D41AB43}"/>
-    <hyperlink ref="G25" r:id="rId92" xr:uid="{89E55572-0304-4BCC-BE99-568E72EDFF0C}"/>
-    <hyperlink ref="G26" r:id="rId93" xr:uid="{980A087E-22CE-4B9D-B75C-1A053CF4E192}"/>
-    <hyperlink ref="G27" r:id="rId94" xr:uid="{C3DCEA69-1368-4865-B7C4-2DAB3BEF4521}"/>
-    <hyperlink ref="G28" r:id="rId95" xr:uid="{EC760423-E41F-4AE0-ACE3-9F13F15E4687}"/>
-    <hyperlink ref="G29" r:id="rId96" xr:uid="{065EFF57-5043-48DA-8C14-5BAE846A1347}"/>
-    <hyperlink ref="H5" r:id="rId97" xr:uid="{A0A77FCC-6E9F-4DDF-99CF-7405F9C9705D}"/>
-    <hyperlink ref="H6" r:id="rId98" xr:uid="{CD9BBF77-8309-4BEC-80B7-012AC8E8DFA0}"/>
-    <hyperlink ref="H7" r:id="rId99" xr:uid="{DEF5098C-CEFC-4516-9F25-C16CB77F3284}"/>
-    <hyperlink ref="H8" r:id="rId100" xr:uid="{D6F08635-202C-447C-90B3-1EE0172BD954}"/>
-    <hyperlink ref="H9" r:id="rId101" xr:uid="{088A9D2F-F275-4D3D-A7C1-55BBD1741E0D}"/>
-    <hyperlink ref="H10" r:id="rId102" xr:uid="{EF0DF1CE-F86A-4D49-B1C9-F3A5E1C578D0}"/>
-    <hyperlink ref="H11" r:id="rId103" xr:uid="{54B0F287-A268-42B0-956E-7DCE2544853D}"/>
-    <hyperlink ref="H12" r:id="rId104" xr:uid="{FB25299B-ECB8-4C78-8B0F-9CD029F5610F}"/>
-    <hyperlink ref="H13" r:id="rId105" xr:uid="{2D496E98-2B72-4DA3-A8BE-0346C7D48A03}"/>
-    <hyperlink ref="H14" r:id="rId106" xr:uid="{43C31856-B44E-4FF3-9FD0-5092B71816CE}"/>
-    <hyperlink ref="H15" r:id="rId107" xr:uid="{A9E2DF98-D6A9-471C-A50C-DB386031B7B9}"/>
-    <hyperlink ref="H16" r:id="rId108" xr:uid="{0B884432-0124-4926-B3C9-894A2AE92E56}"/>
-    <hyperlink ref="H17" r:id="rId109" xr:uid="{261CC7A2-4C81-42DA-9A18-FC1B5F98FCC8}"/>
-    <hyperlink ref="H18" r:id="rId110" display="https://www.downtoearth.org.in/hindistory/governance/%E0%A4%86%E0%A4%9C%E0%A4%BE%E0%A4%A6%E0%A5%80-%E0%A4%95%E0%A4%BE-%E0%A4%B8%E0%A4%82%E0%A4%98%E0%A4%B0%E0%A5%8D%E0%A4%B7-60131" xr:uid="{ECC99108-B9DE-4046-ACC1-0E5AEF87C540}"/>
-    <hyperlink ref="H19" r:id="rId111" display="https://www.downtoearth.org.in/hindistory/health/child-health/%E0%A4%AE%E0%A4%A7%E0%A5%8D%E0%A4%AF-%E0%A4%A6%E0%A5%87%E0%A4%B6-%E0%A4%95-45-00-000-%E0%A4%95%E0%A5%81%E0%A4%AA%E0%A5%8B%E0%A4%B7%E0%A4%BF%E0%A4%A4-%E0%A4%AC%E0%A4%9A%E0%A5%8D%E0%A4%9A%E0%A5%8B%E0%A4%82-%E0%A4%95%E0%A5%80-%E0%A4%A4%E0%A4%B8%E0%A5%8D%E0%A4%B5%E0%A5%80%E0%A4%B0-57608" xr:uid="{0F0C7009-E033-4D85-9D69-AF1FDD5E6E96}"/>
-    <hyperlink ref="H20" r:id="rId112" xr:uid="{2CDAACB5-218E-4051-BD75-FE014D5CD6F9}"/>
+    <hyperlink ref="F5" r:id="rId66" xr:uid="{355C9F80-5851-45EB-AA61-2D400AC39C40}"/>
+    <hyperlink ref="F6" r:id="rId67" xr:uid="{0C0516A7-7AC8-4132-A632-144B988DEDAC}"/>
+    <hyperlink ref="F7" r:id="rId68" xr:uid="{E0F2986D-CA81-4EA1-8548-DC7F377C2E79}"/>
+    <hyperlink ref="F8" r:id="rId69" xr:uid="{67BD70F3-ABE9-4C8F-AFB1-41B6D51FBAF6}"/>
+    <hyperlink ref="F9" r:id="rId70" xr:uid="{1AAEE675-B4FF-4FA3-83FA-7393FFBD697B}"/>
+    <hyperlink ref="G5" r:id="rId71" xr:uid="{363702E4-8A66-4A19-AA8F-679E22E89404}"/>
+    <hyperlink ref="G6" r:id="rId72" xr:uid="{BEDF7C13-C82E-4CB5-8860-6E9C089A3826}"/>
+    <hyperlink ref="G7" r:id="rId73" xr:uid="{C65C518A-17C5-4C37-B156-B294BB7C39DE}"/>
+    <hyperlink ref="G8" r:id="rId74" xr:uid="{1A08BA37-85E0-46EC-BE46-4CFF50561D88}"/>
+    <hyperlink ref="G9" r:id="rId75" xr:uid="{D1A6861C-9A60-441C-ACCE-9DA32723FD25}"/>
+    <hyperlink ref="G10" r:id="rId76" xr:uid="{BE83C08E-9EAE-4B29-B12C-7C6BEA71710E}"/>
+    <hyperlink ref="G11" r:id="rId77" xr:uid="{F9FADDBC-B865-49C2-8DA7-31DD7D450BB6}"/>
+    <hyperlink ref="G12" r:id="rId78" xr:uid="{455C45C1-E21D-47FC-831A-41CDD067DA7F}"/>
+    <hyperlink ref="G13" r:id="rId79" xr:uid="{3DA6D7C1-09B5-49C4-9B34-4316A05F2F32}"/>
+    <hyperlink ref="G14" r:id="rId80" xr:uid="{25178FE7-FA65-4469-B8FB-2CAB8F5A603E}"/>
+    <hyperlink ref="G15" r:id="rId81" xr:uid="{557D08BC-5C21-4FC3-9724-C76098698E3D}"/>
+    <hyperlink ref="G16" r:id="rId82" xr:uid="{9C0B4647-6398-46DE-91C5-D70A157EB87D}"/>
+    <hyperlink ref="G17" r:id="rId83" xr:uid="{EB927B41-C00C-4953-AD42-82B427AD4B72}"/>
+    <hyperlink ref="G18" r:id="rId84" xr:uid="{431D0FB1-AB5E-4AE5-A04A-24C256A2BF31}"/>
+    <hyperlink ref="G19" r:id="rId85" xr:uid="{F7251C95-65F3-4AEE-ABDA-2753B311B594}"/>
+    <hyperlink ref="G20" r:id="rId86" xr:uid="{F35454C0-EC02-4D31-B421-FAC25569AC72}"/>
+    <hyperlink ref="G21" r:id="rId87" xr:uid="{87E4AC5D-2E2F-47CD-9FC0-0E7825DE6414}"/>
+    <hyperlink ref="G22" r:id="rId88" xr:uid="{BF883CF3-071F-4584-A944-B0975E1EED1F}"/>
+    <hyperlink ref="G23" r:id="rId89" xr:uid="{B69207CB-3C13-484E-B116-78D83E9B50AC}"/>
+    <hyperlink ref="G24" r:id="rId90" xr:uid="{434F605D-D946-4CCC-AA04-39966D41AB43}"/>
+    <hyperlink ref="G25" r:id="rId91" xr:uid="{89E55572-0304-4BCC-BE99-568E72EDFF0C}"/>
+    <hyperlink ref="G26" r:id="rId92" xr:uid="{980A087E-22CE-4B9D-B75C-1A053CF4E192}"/>
+    <hyperlink ref="G27" r:id="rId93" xr:uid="{C3DCEA69-1368-4865-B7C4-2DAB3BEF4521}"/>
+    <hyperlink ref="G28" r:id="rId94" xr:uid="{EC760423-E41F-4AE0-ACE3-9F13F15E4687}"/>
+    <hyperlink ref="G29" r:id="rId95" xr:uid="{065EFF57-5043-48DA-8C14-5BAE846A1347}"/>
+    <hyperlink ref="H5" r:id="rId96" xr:uid="{A0A77FCC-6E9F-4DDF-99CF-7405F9C9705D}"/>
+    <hyperlink ref="H6" r:id="rId97" xr:uid="{CD9BBF77-8309-4BEC-80B7-012AC8E8DFA0}"/>
+    <hyperlink ref="H7" r:id="rId98" xr:uid="{DEF5098C-CEFC-4516-9F25-C16CB77F3284}"/>
+    <hyperlink ref="H8" r:id="rId99" xr:uid="{D6F08635-202C-447C-90B3-1EE0172BD954}"/>
+    <hyperlink ref="H9" r:id="rId100" xr:uid="{088A9D2F-F275-4D3D-A7C1-55BBD1741E0D}"/>
+    <hyperlink ref="H10" r:id="rId101" xr:uid="{EF0DF1CE-F86A-4D49-B1C9-F3A5E1C578D0}"/>
+    <hyperlink ref="H11" r:id="rId102" xr:uid="{54B0F287-A268-42B0-956E-7DCE2544853D}"/>
+    <hyperlink ref="H12" r:id="rId103" xr:uid="{FB25299B-ECB8-4C78-8B0F-9CD029F5610F}"/>
+    <hyperlink ref="H13" r:id="rId104" xr:uid="{2D496E98-2B72-4DA3-A8BE-0346C7D48A03}"/>
+    <hyperlink ref="H14" r:id="rId105" xr:uid="{43C31856-B44E-4FF3-9FD0-5092B71816CE}"/>
+    <hyperlink ref="H15" r:id="rId106" xr:uid="{A9E2DF98-D6A9-471C-A50C-DB386031B7B9}"/>
+    <hyperlink ref="H16" r:id="rId107" xr:uid="{0B884432-0124-4926-B3C9-894A2AE92E56}"/>
+    <hyperlink ref="H17" r:id="rId108" xr:uid="{261CC7A2-4C81-42DA-9A18-FC1B5F98FCC8}"/>
+    <hyperlink ref="H18" r:id="rId109" display="https://www.downtoearth.org.in/hindistory/governance/%E0%A4%86%E0%A4%9C%E0%A4%BE%E0%A4%A6%E0%A5%80-%E0%A4%95%E0%A4%BE-%E0%A4%B8%E0%A4%82%E0%A4%98%E0%A4%B0%E0%A5%8D%E0%A4%B7-60131" xr:uid="{ECC99108-B9DE-4046-ACC1-0E5AEF87C540}"/>
+    <hyperlink ref="H19" r:id="rId110" display="https://www.downtoearth.org.in/hindistory/health/child-health/%E0%A4%AE%E0%A4%A7%E0%A5%8D%E0%A4%AF-%E0%A4%A6%E0%A5%87%E0%A4%B6-%E0%A4%95-45-00-000-%E0%A4%95%E0%A5%81%E0%A4%AA%E0%A5%8B%E0%A4%B7%E0%A4%BF%E0%A4%A4-%E0%A4%AC%E0%A4%9A%E0%A5%8D%E0%A4%9A%E0%A5%8B%E0%A4%82-%E0%A4%95%E0%A5%80-%E0%A4%A4%E0%A4%B8%E0%A5%8D%E0%A4%B5%E0%A5%80%E0%A4%B0-57608" xr:uid="{0F0C7009-E033-4D85-9D69-AF1FDD5E6E96}"/>
+    <hyperlink ref="H20" r:id="rId111" xr:uid="{2CDAACB5-218E-4051-BD75-FE014D5CD6F9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId112"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more articles added and side menu bar made to work
</commit_message>
<xml_diff>
--- a/Links.xlsx
+++ b/Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aditya\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1156254A-2492-4D3C-BC0E-8662906BBC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4C979E-0B91-453D-94E5-A5BD4F6620FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0AE215CC-A1AB-4149-94F4-3B8936C851DB}"/>
   </bookViews>
@@ -442,17 +442,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -805,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B6FFBC-4681-4669-B232-AC94051921B9}">
   <dimension ref="A4:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1233,11 +1223,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A4:H29">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A4:H29">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1" xr:uid="{6309066A-7C9F-4DEA-A9DD-A4AF05B10080}"/>

</xml_diff>

<commit_message>
fixed padding bug in footer
</commit_message>
<xml_diff>
--- a/Links.xlsx
+++ b/Links.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aditya\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4C979E-0B91-453D-94E5-A5BD4F6620FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0259E1-A521-4DE7-AEB9-EFD4F674C54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0AE215CC-A1AB-4149-94F4-3B8936C851DB}"/>
   </bookViews>
@@ -795,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B6FFBC-4681-4669-B232-AC94051921B9}">
   <dimension ref="A4:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -995,6 +995,12 @@
       <c r="D11" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1">
+        <v>5</v>
+      </c>
       <c r="G11" s="3" t="s">
         <v>78</v>
       </c>
@@ -1088,6 +1094,9 @@
       </c>
       <c r="B16" s="3" t="s">
         <v>35</v>
+      </c>
+      <c r="C16" s="1">
+        <v>11</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
more articles added with font size changes to fix some bugs
</commit_message>
<xml_diff>
--- a/Links.xlsx
+++ b/Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aditya\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0259E1-A521-4DE7-AEB9-EFD4F674C54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B74825-0532-4ED7-9189-8EF00165BB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0AE215CC-A1AB-4149-94F4-3B8936C851DB}"/>
   </bookViews>
@@ -404,12 +404,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -425,7 +431,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -437,6 +443,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -793,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B6FFBC-4681-4669-B232-AC94051921B9}">
-  <dimension ref="A4:H29"/>
+  <dimension ref="A4:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1163,6 +1172,9 @@
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="B20" s="1">
+        <v>15</v>
+      </c>
       <c r="D20" s="3" t="s">
         <v>62</v>
       </c>
@@ -1186,10 +1198,13 @@
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>17</v>
+      </c>
       <c r="D22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="5" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1202,6 +1217,9 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D24" s="1">
+        <v>19</v>
+      </c>
       <c r="G24" s="3" t="s">
         <v>91</v>
       </c>
@@ -1229,6 +1247,11 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G29" s="3" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G30" s="1">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>